<commit_message>
change how the protocol works; make it simpler
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="44">
   <si>
     <t>Message type</t>
   </si>
@@ -46,15 +46,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Padding is only needed to work around specific browser problems, and maybe annoying proxies.</t>
-  </si>
-  <si>
-    <t>gimme is really only about instructing the server about how the client wants this transport to be used; waiting for a "gimme" from the server before client can send any boxes would introduce a round trip.</t>
-  </si>
-  <si>
-    <t>gimme, waitOnConn</t>
   </si>
   <si>
     <t>C2S HTTP: sack_and_close to use the transport for "upload only" (it wants the request closed ASAP). 
@@ -69,9 +60,6 @@
     <t>c_c, no_such_stream</t>
   </si>
   <si>
-    <t>hello is used by the client to identify itself to the server, and set critical transport parameters</t>
-  </si>
-  <si>
     <t>c_c, could_not_attach</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>c_c, invalid_arguments</t>
   </si>
   <si>
-    <t>C2S HTTP: If the server sent corrupt frames, just make a new C2S HTTP request.</t>
-  </si>
-  <si>
     <t>Y / N indicates whether this message is part of the spec for this direction (C2S/S2C) and mode (HTTP/Sock)</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
     <t>my_last_frame</t>
   </si>
   <si>
-    <t>Client cannot be overloaded</t>
-  </si>
-  <si>
     <t>gimme_sack_and_close</t>
   </si>
   <si>
@@ -145,13 +127,38 @@
   </si>
   <si>
     <t>Both parties send boxes - this is the whole point.</t>
+  </si>
+  <si>
+    <t>gimme_boxes is really only about instructing the server about how the client wants this transport to be used; waiting for a "gimme_boxes" from the server before client can send any boxes would introduce a round trip.</t>
+  </si>
+  <si>
+    <t>gimme_boxes, waitOnConn</t>
+  </si>
+  <si>
+    <t>helloData: {"t": transportType, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
+Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
+  </si>
+  <si>
+    <t>Padding is only needed to work around specific browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
+  </si>
+  <si>
+    <t>This means server closed the connection because it is overloaded. Client cannot be overloaded.</t>
+  </si>
+  <si>
+    <t>This means the actual extraction of frame-strings from the octetstream failed. If client received corrupt frames, just make a new request.</t>
+  </si>
+  <si>
+    <t>This means the JSON in some frame could not be parsed. If client received corrupt frames, just make a new request.</t>
+  </si>
+  <si>
+    <t>If server send this, client sent 'hello', 'gimme_boxes', 'start_timestamps', or 'stop_timestamps' with invalid arguments. Because server doesn't send any frames that have parameters, client never sends invalid_arguments.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,12 +167,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,261 +202,23 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -890,33 +664,33 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="6.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="125.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="127.85546875" style="2" customWidth="1"/>
     <col min="7" max="9" width="94" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1">
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -939,7 +713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1">
+    <row r="5" spans="1:6" ht="33" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -956,10 +730,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32.25" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -976,52 +750,52 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="36.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="52.5" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="74.25" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -1036,12 +810,12 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -1058,7 +832,7 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -1073,12 +847,12 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -1093,12 +867,12 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="27" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -1113,12 +887,12 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="21.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -1133,12 +907,12 @@
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>8</v>
@@ -1157,7 +931,7 @@
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -1172,12 +946,12 @@
         <v>5</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -1192,18 +966,18 @@
         <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>5</v>
@@ -1212,18 +986,18 @@
         <v>5</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>5</v>
@@ -1232,18 +1006,18 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>
@@ -1252,18 +1026,18 @@
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>5</v>
@@ -1272,12 +1046,12 @@
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1292,7 +1066,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update docs/protocol.xlsx; fix an import in link.py
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>Message type</t>
   </si>
@@ -48,48 +48,15 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>C2S HTTP: sack_and_close to use the transport for "upload only" (it wants the request closed ASAP). 
-C2S Socket: again, to use the transport for "upload only" if for some reason using a second (web)socket for upload is useful
-S2C HTTP: no, because asking the client to abort() the request means that they have to trash the TCP connection. Plus, they would have to make another HTTP request to send the SACK.
-S2C Socket: yes, because it's reasonable to ask the client to close a two-way socket connection so that the client holds onto the TIME_WAIT</t>
-  </si>
-  <si>
-    <t>c_c means close_connection</t>
-  </si>
-  <si>
-    <t>c_c, no_such_stream</t>
-  </si>
-  <si>
-    <t>c_c, could_not_attach</t>
-  </si>
-  <si>
     <t>This error is a possible response to hello</t>
   </si>
   <si>
-    <t>c_c, acked_unsent_boxes</t>
-  </si>
-  <si>
     <t>Only the server sends acked_unsent_boxes. If the client thinks server sent a bad SACK, it should send 'reset'</t>
   </si>
   <si>
-    <t>c_c, frame_corruption</t>
-  </si>
-  <si>
-    <t>c_c, intraframe_corruption</t>
-  </si>
-  <si>
-    <t>c_c, invalid_arguments</t>
-  </si>
-  <si>
     <t>Y / N indicates whether this message is part of the spec for this direction (C2S/S2C) and mode (HTTP/Sock)</t>
   </si>
   <si>
-    <t>c_c, overloaded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There's a difference  between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, </t>
-  </si>
-  <si>
     <t>"</t>
   </si>
   <si>
@@ -108,9 +75,6 @@
     <t>start_timestamps, connnectionNumber, interval, howMany</t>
   </si>
   <si>
-    <t xml:space="preserve">Timestamp feature is only used by clients to determine if streaming connection is being buffered, and as a feature to ask for NOOPs to prevent the connection from being closed. </t>
-  </si>
-  <si>
     <t>stop_timestamps, connectionNumber</t>
   </si>
   <si>
@@ -124,12 +88,6 @@
   </si>
   <si>
     <t>boxes, boxes</t>
-  </si>
-  <si>
-    <t>Both parties send boxes - this is the whole point.</t>
-  </si>
-  <si>
-    <t>gimme_boxes is really only about instructing the server about how the client wants this transport to be used; waiting for a "gimme_boxes" from the server before client can send any boxes would introduce a round trip.</t>
   </si>
   <si>
     <t>gimme_boxes, waitOnConn</t>
@@ -139,12 +97,6 @@
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
   </si>
   <si>
-    <t>Padding is only needed to work around specific browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
-  </si>
-  <si>
-    <t>This means server closed the connection because it is overloaded. Client cannot be overloaded.</t>
-  </si>
-  <si>
     <t>This means the actual extraction of frame-strings from the octetstream failed. If client received corrupt frames, just make a new request.</t>
   </si>
   <si>
@@ -152,6 +104,65 @@
   </si>
   <si>
     <t>If server send this, client sent 'hello', 'gimme_boxes', 'start_timestamps', or 'stop_timestamps' with invalid arguments. Because server doesn't send any frames that have parameters, client never sends invalid_arguments.</t>
+  </si>
+  <si>
+    <t>Both parties send boxes - this is the whole point of Minerva.</t>
+  </si>
+  <si>
+    <t>This is a marker that says that this is the last frame I will ever send over this transport.</t>
+  </si>
+  <si>
+    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip.</t>
+  </si>
+  <si>
+    <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
+  </si>
+  <si>
+    <t>Clients need timestamps to determine if a streaming connection is being buffered, and can also use them as NOOPs to prevent a connection from closing.</t>
+  </si>
+  <si>
+    <t>There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch.</t>
+  </si>
+  <si>
+    <t>This means server closed the transport because it is overloaded. Client cannot be overloaded.</t>
+  </si>
+  <si>
+    <t>c_t, no_such_stream</t>
+  </si>
+  <si>
+    <t>c_t, could_not_attach</t>
+  </si>
+  <si>
+    <t>c_t, acked_unsent_boxes</t>
+  </si>
+  <si>
+    <t>c_t, frame_corruption</t>
+  </si>
+  <si>
+    <t>c_t, intraframe_corruption</t>
+  </si>
+  <si>
+    <t>c_t, invalid_arguments</t>
+  </si>
+  <si>
+    <t>c_t, overloaded</t>
+  </si>
+  <si>
+    <t>c_t means close_transport</t>
+  </si>
+  <si>
+    <t>Idea: maybe distinct 'goodbye' and 'reset'? Maybe a 'please_send_sack' if either party urgently wants a sack to reduce its memory use?</t>
+  </si>
+  <si>
+    <t>you_close_it</t>
+  </si>
+  <si>
+    <t>This is only for the client to tell the server what it wants.
+C2S HTTP: sack_and_close to use the transport for "upload only" (it wants the request closed ASAP). 
+C2S Socket: again, to use the transport for "upload only" if for some reason using a second (web)socket for upload is useful</t>
+  </si>
+  <si>
+    <t>This is useful when one side wants to close the connection, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
   </si>
 </sst>
 </file>
@@ -218,77 +229,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -661,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -678,19 +619,19 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1">
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1">
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1">
-      <c r="B3" s="1" t="s">
-        <v>22</v>
+    <row r="1" spans="1:6" ht="22.5" customHeight="1">
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+      <c r="F2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" customHeight="1">
+      <c r="F3" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -730,10 +671,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="32.25" customHeight="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -750,12 +691,12 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="36.75" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -770,12 +711,12 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="52.5" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="38.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -787,15 +728,15 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -810,12 +751,12 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -828,11 +769,14 @@
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -847,12 +791,12 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="31.5" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -867,12 +811,12 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="27" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -887,12 +831,12 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="21.75" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -907,12 +851,12 @@
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>8</v>
@@ -927,11 +871,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -946,12 +909,12 @@
         <v>5</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -966,12 +929,12 @@
         <v>5</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -986,12 +949,12 @@
         <v>5</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -1006,12 +969,12 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1026,12 +989,12 @@
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1046,12 +1009,12 @@
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1066,15 +1029,20 @@
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:A1048576 B4:B1048576 C1:XFD1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add lots of untested code
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
   <si>
     <t>Message type</t>
   </si>
@@ -125,30 +125,6 @@
   </si>
   <si>
     <t>This means server closed the transport because it is overloaded. Client cannot be overloaded.</t>
-  </si>
-  <si>
-    <t>c_t, no_such_stream</t>
-  </si>
-  <si>
-    <t>c_t, could_not_attach</t>
-  </si>
-  <si>
-    <t>c_t, acked_unsent_boxes</t>
-  </si>
-  <si>
-    <t>c_t, frame_corruption</t>
-  </si>
-  <si>
-    <t>c_t, intraframe_corruption</t>
-  </si>
-  <si>
-    <t>c_t, invalid_arguments</t>
-  </si>
-  <si>
-    <t>c_t, overloaded</t>
-  </si>
-  <si>
-    <t>c_t means close_transport</t>
   </si>
   <si>
     <t>Idea: maybe distinct 'goodbye' and 'reset'? Maybe a 'please_send_sack' if either party urgently wants a sack to reduce its memory use?</t>
@@ -163,6 +139,36 @@
   </si>
   <si>
     <t>This is useful when one side wants to close the connection, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
+  </si>
+  <si>
+    <t>t_k, no_such_stream</t>
+  </si>
+  <si>
+    <t>t_k, could_not_attach</t>
+  </si>
+  <si>
+    <t>t_k, acked_unsent_boxes</t>
+  </si>
+  <si>
+    <t>t_k, frame_corruption</t>
+  </si>
+  <si>
+    <t>t_k, intraframe_corruption</t>
+  </si>
+  <si>
+    <t>t_k, invalid_arguments</t>
+  </si>
+  <si>
+    <t>t_k, overloaded</t>
+  </si>
+  <si>
+    <t>t_k means transport_kill</t>
+  </si>
+  <si>
+    <t>t_k, brb, seconds</t>
+  </si>
+  <si>
+    <t>Often called when the server is shutting down</t>
   </si>
 </sst>
 </file>
@@ -229,7 +235,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -605,7 +639,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -626,7 +660,7 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1">
@@ -731,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
@@ -873,7 +907,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -888,13 +922,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -914,7 +948,7 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -934,7 +968,7 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -954,7 +988,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -974,7 +1008,7 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -994,7 +1028,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1014,7 +1048,7 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1032,17 +1066,37 @@
         <v>35</v>
       </c>
     </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576 B4:B1048576 C1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add CsrfTransportFirewall; make fix to NoopTransportFirewall; update protocol.xlsx; copy dummies from test_link to test_newlink
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -235,35 +235,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -639,7 +611,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -1066,7 +1038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1">
+    <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1093,10 +1065,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576 B4:B1048576 C1:XFD1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add FakeReactor; start work on more tests; other fixes
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -138,9 +138,6 @@
 C2S Socket: again, to use the transport for "upload only" if for some reason using a second (web)socket for upload is useful</t>
   </si>
   <si>
-    <t>This is useful when one side wants to close the connection, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
-  </si>
-  <si>
     <t>t_k, no_such_stream</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>Often called when the server is shutting down</t>
+  </si>
+  <si>
+    <t>This is useful when one side wants to close the transport, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
   </si>
 </sst>
 </file>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -632,7 +632,7 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1">
@@ -894,13 +894,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1040,22 +1040,22 @@
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">

</xml_diff>

<commit_message>
add TestEnsureNonNegInt32; work on sockettransport
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="12855"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,10 +93,6 @@
     <t>gimme_boxes, waitOnConn</t>
   </si>
   <si>
-    <t>helloData: {"t": transportType, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
-Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
-  </si>
-  <si>
     <t>This means the actual extraction of frame-strings from the octetstream failed. If client received corrupt frames, just make a new request.</t>
   </si>
   <si>
@@ -169,6 +165,10 @@
   </si>
   <si>
     <t>This is useful when one side wants to close the transport, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
+  </si>
+  <si>
+    <t>helloData: {"v: protocolVersion, "t": transportType, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
+Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -632,12 +632,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -660,7 +660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="33" customHeight="1">
+    <row r="5" spans="1:6" ht="38.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -677,7 +677,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -697,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5">
@@ -717,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -737,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
@@ -757,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -777,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -837,7 +837,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
@@ -879,7 +879,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -894,13 +894,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -975,12 +975,12 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -995,12 +995,12 @@
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1015,12 +1015,12 @@
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1035,32 +1035,32 @@
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ensureNonNegInt32 -> ensureNonNegIntLimit; more work on socket transport and protocol.xlsx
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -167,7 +167,7 @@
     <t>This is useful when one side wants to close the transport, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
   </si>
   <si>
-    <t>helloData: {"v: protocolVersion, "t": transportType, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
+    <t>helloData: {"n": connectionNumber, "v: protocolVersion, "t": transportType, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
   </si>
 </sst>
@@ -611,7 +611,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>

</xml_diff>

<commit_message>
more tests; update protocol.xlsx
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -117,9 +117,6 @@
     <t>Clients need timestamps to determine if a streaming connection is being buffered, and can also use them as NOOPs to prevent a connection from closing.</t>
   </si>
   <si>
-    <t>There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch.</t>
-  </si>
-  <si>
     <t>This means server closed the transport because it is overloaded. Client cannot be overloaded.</t>
   </si>
   <si>
@@ -169,6 +166,21 @@
   <si>
     <t>helloData: {"n": connectionNumber, "v: protocolVersion, "t": transportType, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>How to signify that this is a "new stream"? Is connectionNumber == 0 okay? (when this connection fails things get a bit tricky)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -610,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -632,12 +644,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -677,7 +689,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -737,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
@@ -879,7 +891,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -894,13 +906,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -920,7 +932,7 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -940,7 +952,7 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -960,7 +972,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -980,7 +992,7 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1000,7 +1012,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1020,7 +1032,7 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1035,32 +1047,32 @@
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
isFirstTransport -> requestNewStream; update spec
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -90,13 +90,7 @@
     <t>gimme_boxes, waitOnConn</t>
   </si>
   <si>
-    <t>This means the actual extraction of frame-strings from the octetstream failed. If client received corrupt frames, just make a new request.</t>
-  </si>
-  <si>
     <t>This means the JSON in some frame could not be parsed. If client received corrupt frames, just make a new request.</t>
-  </si>
-  <si>
-    <t>If server send this, client sent 'hello', 'gimme_boxes', 'start_timestamps', or 'stop_timestamps' with invalid arguments. Because server doesn't send any frames that have parameters, client never sends invalid_arguments.</t>
   </si>
   <si>
     <t>Both parties send boxes - this is the whole point of Minerva.</t>
@@ -143,9 +137,6 @@
     <t>t_k, intraframe_corruption</t>
   </si>
   <si>
-    <t>t_k, invalid_arguments</t>
-  </si>
-  <si>
     <t>t_k, overloaded</t>
   </si>
   <si>
@@ -159,10 +150,6 @@
   </si>
   <si>
     <t>This is useful when one side wants to close the transport, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
-  </si>
-  <si>
-    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
-Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
   </si>
   <si>
     <t>stop_timestamps, transportNumber</t>
@@ -181,6 +168,19 @@
       </rPr>
       <t>How to signify that this is a "new stream"? Is transportNumber == 0 okay? (when this connection fails things get a bit tricky)</t>
     </r>
+  </si>
+  <si>
+    <t>t_k, tk_invalid_frame_type_or_arguments</t>
+  </si>
+  <si>
+    <t>If server send this, client sent 'hello', 'gimme_boxes', 'start_timestamps', or 'stop_timestamps' with invalid arguments, or a frame with an unexpected type was received. Should client ever send invalid_arguments? Probably not; client can just ignore frames it doesn't understand.</t>
+  </si>
+  <si>
+    <t>This means the actual extraction of frame-strings from the octetstream failed. If client received corrupt frames, just make a new transport.</t>
+  </si>
+  <si>
+    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
+Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -658,12 +658,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -703,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -723,7 +723,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5">
@@ -743,7 +743,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -763,7 +763,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
@@ -783,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -803,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -863,12 +863,12 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -920,13 +920,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -1001,12 +1001,12 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1021,12 +1021,12 @@
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1041,12 +1041,12 @@
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1061,12 +1061,12 @@
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
@@ -1081,12 +1081,12 @@
         <v>5</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on memory consumption attack prevention ; minor cleanups and fixes
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -87,9 +87,6 @@
     <t>boxes, boxes</t>
   </si>
   <si>
-    <t>gimme_boxes, waitOnConn</t>
-  </si>
-  <si>
     <t>This means the JSON in some frame could not be parsed. If client received corrupt frames, just make a new request.</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>This is a marker that says that this is the last frame I will ever send over this transport.</t>
-  </si>
-  <si>
-    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip.</t>
   </si>
   <si>
     <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
@@ -155,21 +149,6 @@
     <t>stop_timestamps, transportNumber</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>How to signify that this is a "new stream"? Is transportNumber == 0 okay? (when this connection fails things get a bit tricky)</t>
-    </r>
-  </si>
-  <si>
     <t>t_k, tk_invalid_frame_type_or_arguments</t>
   </si>
   <si>
@@ -181,6 +160,15 @@
   <si>
     <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
+  </si>
+  <si>
+    <t>gimme_boxes, waitOnTransport</t>
+  </si>
+  <si>
+    <t>There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch.</t>
+  </si>
+  <si>
+    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If waitOnTransport == -1, give client boxes immediately, else, wait for transport #&lt;waitOnTransport&gt; to close first.</t>
   </si>
 </sst>
 </file>
@@ -247,21 +235,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -636,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -658,12 +632,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -703,7 +677,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -723,12 +697,12 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25.5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -743,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -763,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
@@ -783,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -803,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
@@ -863,12 +837,12 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -905,7 +879,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -920,13 +894,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -946,7 +920,7 @@
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -966,7 +940,7 @@
     </row>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -986,7 +960,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -1001,12 +975,12 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1021,12 +995,12 @@
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1041,12 +1015,12 @@
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1061,12 +1035,12 @@
         <v>5</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
@@ -1081,20 +1055,20 @@
         <v>5</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576 B4:B1048576 C1:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
make start= to iterItems optional; update protocol.xlsx to match code
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
   <si>
     <t>Message type</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Clients need timestamps to determine if a streaming connection is being buffered, and can also use them as NOOPs to prevent a connection from closing.</t>
-  </si>
-  <si>
-    <t>This means server closed the transport because it is overloaded. Client cannot be overloaded.</t>
   </si>
   <si>
     <t>Idea: maybe distinct 'goodbye' and 'reset'? Maybe a 'please_send_sack' if either party urgently wants a sack to reduce its memory use?</t>
@@ -116,12 +113,6 @@
 C2S Socket: again, to use the transport for "upload only" if for some reason using a second (web)socket for upload is useful</t>
   </si>
   <si>
-    <t>t_k, no_such_stream</t>
-  </si>
-  <si>
-    <t>t_k, could_not_attach</t>
-  </si>
-  <si>
     <t>t_k, acked_unsent_boxes</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>t_k, intraframe_corruption</t>
   </si>
   <si>
-    <t>t_k, overloaded</t>
-  </si>
-  <si>
     <t>t_k means transport_kill</t>
   </si>
   <si>
@@ -147,9 +135,6 @@
   </si>
   <si>
     <t>stop_timestamps, transportNumber</t>
-  </si>
-  <si>
-    <t>t_k, tk_invalid_frame_type_or_arguments</t>
   </si>
   <si>
     <t>If server send this, client sent 'hello', 'gimme_boxes', 'start_timestamps', or 'stop_timestamps' with invalid arguments, or a frame with an unexpected type was received. Should client ever send invalid_arguments? Probably not; client can just ignore frames it doesn't understand.</t>
@@ -169,6 +154,12 @@
   </si>
   <si>
     <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If waitOnTransport == -1, give client boxes immediately, else, wait for transport #&lt;waitOnTransport&gt; to close first.</t>
+  </si>
+  <si>
+    <t>t_k, invalid_frame_type_or_arguments</t>
+  </si>
+  <si>
+    <t>t_k, tk_stream_attach_failure</t>
   </si>
 </sst>
 </file>
@@ -610,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -632,12 +623,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -677,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -702,7 +693,7 @@
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -717,7 +708,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -737,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
@@ -842,7 +833,7 @@
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -879,7 +870,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -894,13 +885,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -918,29 +909,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -960,7 +932,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -975,12 +947,12 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1000,7 +972,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1015,32 +987,13 @@
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
@@ -1055,12 +1008,12 @@
         <v>5</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a lot of checks (incl. min/max arg checking) ; update docs/protocol.xlsx
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -66,12 +66,6 @@
     <t>gimme_sack_and_close</t>
   </si>
   <si>
-    <t>reset</t>
-  </si>
-  <si>
-    <t>sack</t>
-  </si>
-  <si>
     <t>start_timestamps, connnectionNumber, interval, howMany</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>t_k, tk_stream_attach_failure</t>
+  </si>
+  <si>
+    <t>sack, seqNum, sackedList</t>
+  </si>
+  <si>
+    <t>reset, unicodeReason</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:F24"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -623,12 +623,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -668,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -688,27 +688,27 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -728,27 +728,27 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -768,12 +768,12 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -788,12 +788,12 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -808,12 +808,12 @@
         <v>5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -828,12 +828,12 @@
         <v>8</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>8</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -885,13 +885,13 @@
         <v>5</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -912,7 +912,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -947,12 +947,12 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -967,12 +967,12 @@
         <v>5</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -987,13 +987,13 @@
         <v>5</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
@@ -1008,12 +1008,12 @@
         <v>5</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update minervasite to make more sense; fix a lot of comments; add more TODOs to README; add advise_connect_bulk_transport to protocol.xlsx
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
   <si>
     <t>Message type</t>
   </si>
@@ -24,13 +24,7 @@
     <t>C2S HTTP</t>
   </si>
   <si>
-    <t>C2S Sock</t>
-  </si>
-  <si>
     <t>S2C HTTP</t>
-  </si>
-  <si>
-    <t>S2C Sock</t>
   </si>
   <si>
     <t>Y</t>
@@ -107,19 +101,7 @@
 C2S Socket: again, to use the transport for "upload only" if for some reason using a second (web)socket for upload is useful</t>
   </si>
   <si>
-    <t>t_k, acked_unsent_boxes</t>
-  </si>
-  <si>
-    <t>t_k, frame_corruption</t>
-  </si>
-  <si>
-    <t>t_k, intraframe_corruption</t>
-  </si>
-  <si>
     <t>t_k means transport_kill</t>
-  </si>
-  <si>
-    <t>t_k, brb, seconds</t>
   </si>
   <si>
     <t>Often called when the server is shutting down</t>
@@ -144,12 +126,6 @@
     <t>There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch.</t>
   </si>
   <si>
-    <t>t_k, invalid_frame_type_or_arguments</t>
-  </si>
-  <si>
-    <t>t_k, tk_stream_attach_failure</t>
-  </si>
-  <si>
     <t>sack, seqNum, sackedList</t>
   </si>
   <si>
@@ -160,6 +136,36 @@
   </si>
   <si>
     <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != -1, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.</t>
+  </si>
+  <si>
+    <t>tk_stream_attach_failure</t>
+  </si>
+  <si>
+    <t>tk_acked_unsent_boxes</t>
+  </si>
+  <si>
+    <t>tk_frame_corruption</t>
+  </si>
+  <si>
+    <t>tk_intraframe_corruption</t>
+  </si>
+  <si>
+    <t>tk_invalid_frame_type_or_arguments</t>
+  </si>
+  <si>
+    <t>tk_brb, seconds</t>
+  </si>
+  <si>
+    <t>S2C Socket-like</t>
+  </si>
+  <si>
+    <t>C2S Socket-like</t>
+  </si>
+  <si>
+    <t>advise_connect_bulk_transport</t>
+  </si>
+  <si>
+    <t>Server indicates that client should try to establish an S2C transport more suitable for bulk transport. TODO: define this more</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -599,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -618,17 +638,17 @@
   <sheetData>
     <row r="1" spans="1:6" ht="22.5" customHeight="1">
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -639,385 +659,404 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" customHeight="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576 B4:B1048576 C1:XFD1048576">
+  <conditionalFormatting sqref="B1:XFD1048576 A1:A25 A27:A1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add some comments about future protocol changes; minor optimizations by reducing use of exceptions
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -66,9 +66,6 @@
     <t>Either party can reset if they've given up on this stream</t>
   </si>
   <si>
-    <t>Both parties need to sack early and sack often</t>
-  </si>
-  <si>
     <t>timestamp, timestamp_sequence_number</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Often called when the server is shutting down</t>
   </si>
   <si>
-    <t>This is useful when one side wants to close the transport, but throw the TIME_WAIT state to the other side. Only server can ask client to do this.</t>
-  </si>
-  <si>
     <t>stop_timestamps, transportNumber</t>
   </si>
   <si>
@@ -166,6 +160,12 @@
   </si>
   <si>
     <t>Server indicates that client should try to establish an S2C transport more suitable for bulk transport. TODO: define this more</t>
+  </si>
+  <si>
+    <t>This is useful when one side wants the other to initiate the active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). Only server can ask client to do this. If you_close_it is sent over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
+  </si>
+  <si>
+    <t>Both parties need to sack often to free memory in their peer's box queue</t>
   </si>
 </sst>
 </file>
@@ -232,21 +232,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -621,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -643,12 +629,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -659,13 +645,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -688,7 +674,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -708,12 +694,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -728,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -748,12 +734,12 @@
         <v>6</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -768,7 +754,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -788,12 +774,12 @@
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -813,7 +799,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -828,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
@@ -848,12 +834,12 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -873,7 +859,7 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -888,9 +874,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1">
+    <row r="16" spans="1:6" ht="40.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -905,13 +891,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -932,7 +918,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -952,7 +938,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -967,12 +953,12 @@
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -987,12 +973,12 @@
         <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -1007,12 +993,12 @@
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -1027,12 +1013,12 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1047,12 +1033,12 @@
         <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement test_gimmeBoxes*; change protocol to use `null`/`None` instead of -1 in gimme_boxes frame
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -129,9 +129,6 @@
     <t>gimme_boxes, succeedsTransport</t>
   </si>
   <si>
-    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != -1, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.</t>
-  </si>
-  <si>
     <t>tk_stream_attach_failure</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>Both parties need to sack often to free memory in their peer's box queue</t>
+  </si>
+  <si>
+    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -645,13 +645,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -714,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="38.25">
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
@@ -891,13 +891,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -918,7 +918,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -1018,22 +1018,22 @@
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">

</xml_diff>

<commit_message>
change how the protocol works (use C2S you_close_it to request that server close an HTTP request); add test_you_close_it_forbidden
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
   <si>
     <t>Message type</t>
   </si>
@@ -57,9 +57,6 @@
     <t>my_last_frame</t>
   </si>
   <si>
-    <t>gimme_sack_and_close</t>
-  </si>
-  <si>
     <t>start_timestamps, connnectionNumber, interval, howMany</t>
   </si>
   <si>
@@ -91,11 +88,6 @@
   </si>
   <si>
     <t>you_close_it</t>
-  </si>
-  <si>
-    <t>This is only for the client to tell the server what it wants.
-C2S HTTP: sack_and_close to use the transport for "upload only" (it wants the request closed ASAP). 
-C2S Socket: again, to use the transport for "upload only" if for some reason using a second (web)socket for upload is useful</t>
   </si>
   <si>
     <t>t_k means transport_kill</t>
@@ -159,13 +151,14 @@
     <t>Server indicates that client should try to establish an S2C transport more suitable for bulk transport. TODO: define this more</t>
   </si>
   <si>
-    <t>This is useful when one side wants the other to initiate the active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). Only server can ask client to do this. If you_close_it is sent over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
-  </si>
-  <si>
     <t>Both parties need to sack often to free memory in their peer's box queue</t>
   </si>
   <si>
     <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)
+In C2S context: (only allowed for HTTP) client wants server to finish the HTTP request ASAP. This does not imply connection close. This is useful for "upload only" HTTP transports, where the client uploads data (box/boxes frame) and then sends you_close_it to get the request closed. </t>
   </si>
 </sst>
 </file>
@@ -607,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -629,12 +622,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -645,13 +638,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -674,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -694,12 +687,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -714,32 +707,13 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="38.25">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75"/>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -754,7 +728,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
@@ -774,12 +748,12 @@
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -794,12 +768,12 @@
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -814,12 +788,12 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -834,12 +808,12 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -859,7 +833,7 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -874,9 +848,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="40.5" customHeight="1">
+    <row r="16" spans="1:6" ht="66" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -897,7 +871,7 @@
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -918,7 +892,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -938,7 +912,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -953,12 +927,12 @@
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -973,12 +947,12 @@
         <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -993,12 +967,12 @@
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -1013,12 +987,12 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1033,12 +1007,12 @@
         <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove my_last_frame from everywhere
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
   <si>
     <t>Message type</t>
   </si>
@@ -54,9 +54,6 @@
     <t>"</t>
   </si>
   <si>
-    <t>my_last_frame</t>
-  </si>
-  <si>
     <t>start_timestamps, connnectionNumber, interval, howMany</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>Both parties send boxes - this is the whole point of Minerva.</t>
-  </si>
-  <si>
-    <t>This is a marker that says that this is the last frame I will ever send over this transport.</t>
   </si>
   <si>
     <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
@@ -601,7 +595,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A10" sqref="A10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -622,12 +616,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -638,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -667,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -687,12 +681,12 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -707,13 +701,13 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75"/>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -728,32 +722,13 @@
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -768,12 +743,12 @@
         <v>3</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -788,12 +763,12 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -808,12 +783,12 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -833,7 +808,7 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -850,7 +825,7 @@
     </row>
     <row r="16" spans="1:6" ht="66" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -865,13 +840,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -892,7 +867,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -912,7 +887,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -927,12 +902,12 @@
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -947,12 +922,12 @@
         <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -967,12 +942,12 @@
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -987,12 +962,12 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1007,12 +982,12 @@
         <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move code around; add comments
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -75,9 +75,6 @@
     <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
   </si>
   <si>
-    <t>Clients need timestamps to determine if a streaming connection is being buffered, and can also use them as NOOPs to prevent a connection from closing.</t>
-  </si>
-  <si>
     <t>Idea: maybe distinct 'goodbye' and 'reset'? Maybe a 'please_send_sack' if either party urgently wants a sack to reduce its memory use?</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   <si>
     <t xml:space="preserve">In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)
 In C2S context: (only allowed for HTTP) client wants server to finish the HTTP request ASAP. This does not imply connection close. This is useful for "upload only" HTTP transports, where the client uploads data (box/boxes frame) and then sends you_close_it to get the request closed. </t>
+  </si>
+  <si>
+    <t>Clients need timestamps to determine if a streaming connection is being buffered, and can also use them as NOOPs to prevent a connection from closing. Or use them as an "please send me an initial message" to determine how long it really took to open the transport.</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -616,12 +616,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -632,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -686,7 +686,7 @@
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75"/>
@@ -728,7 +728,7 @@
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -763,10 +763,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -783,12 +783,12 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="16" spans="1:6" ht="66" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -840,13 +840,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -867,7 +867,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -902,12 +902,12 @@
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -942,12 +942,12 @@
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -962,32 +962,32 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change how reset works; rearrange tests
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -106,9 +106,6 @@
     <t>sack, seqNum, sackedList</t>
   </si>
   <si>
-    <t>reset, unicodeReason</t>
-  </si>
-  <si>
     <t>gimme_boxes, succeedsTransport</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Clients need timestamps to determine if a streaming connection is being buffered, and can also use them as NOOPs to prevent a connection from closing. Or use them as an "please send me an initial message" to determine how long it really took to open the transport.</t>
+  </si>
+  <si>
+    <t>reset, unicodeReason, applicationLevel?</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -632,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75"/>
@@ -728,7 +728,7 @@
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
@@ -783,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
@@ -840,13 +840,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -867,7 +867,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -967,22 +967,22 @@
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">

</xml_diff>

<commit_message>
update protocol to mention yet-unimplemented useMyTcpAcks
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -96,10 +96,6 @@
     <t>This means the actual extraction of frame-strings from the octetstream failed. If client received corrupt frames, just make a new transport.</t>
   </si>
   <si>
-    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce}
-Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
-  </si>
-  <si>
     <t>There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch.</t>
   </si>
   <si>
@@ -153,6 +149,10 @@
   </si>
   <si>
     <t>reset, unicodeReason, applicationLevel?</t>
+  </si>
+  <si>
+    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks}
+Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
   </si>
 </sst>
 </file>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -621,7 +621,7 @@
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1">
       <c r="F3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1">
@@ -632,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -686,7 +686,7 @@
     </row>
     <row r="7" spans="1:6" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75"/>
@@ -728,7 +728,7 @@
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1">
@@ -783,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
@@ -840,13 +840,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -867,7 +867,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -967,22 +967,22 @@
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">

</xml_diff>

<commit_message>
write about pipelining; fix protocol.xlsx to mention you_close_it is allowed for C2S HTTP
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -828,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
work on flashtest; refactor tests a bit; other changes
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -152,7 +152,7 @@
   </si>
   <si>
     <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks}
-Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters</t>
+Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -644,7 +644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="38.25" customHeight="1">
+    <row r="5" spans="1:6" ht="50.25" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fix behavior for SocketTransport.connectionLost; add TODO to protocol.xlsx; clean up 'is not' code
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -138,9 +138,6 @@
     <t>Both parties need to sack often to free memory in their peer's box queue</t>
   </si>
   <si>
-    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.</t>
-  </si>
-  <si>
     <t xml:space="preserve">In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)
 In C2S context: (only allowed for HTTP) client wants server to finish the HTTP request ASAP. This does not imply connection close. This is useful for "upload only" HTTP transports, where the client uploads data (box/boxes frame) and then sends you_close_it to get the request closed. </t>
   </si>
@@ -153,6 +150,9 @@
   <si>
     <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks}
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
+  </si>
+  <si>
+    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed. XXX TODO: Why is gimme_boxes not part of the hello frame?</t>
   </si>
 </sst>
 </file>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1">
@@ -701,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75"/>
@@ -728,7 +728,7 @@
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -783,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
@@ -840,7 +840,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1"/>

</xml_diff>

<commit_message>
don't allow you_close_it for C2S HTTP. you_close_it will be the default behavior if client doesn't send gimme_boxes.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11310"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144315"/>
 </workbook>
 </file>
 
@@ -138,10 +138,6 @@
     <t>Both parties need to sack often to free memory in their peer's box queue</t>
   </si>
   <si>
-    <t xml:space="preserve">In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)
-In C2S context: (only allowed for HTTP) client wants server to finish the HTTP request ASAP. This does not imply connection close. This is useful for "upload only" HTTP transports, where the client uploads data (box/boxes frame) and then sends you_close_it to get the request closed. </t>
-  </si>
-  <si>
     <t>Clients need timestamps to determine if a streaming connection is being buffered, and can also use them as NOOPs to prevent a connection from closing. Or use them as an "please send me an initial message" to determine how long it really took to open the transport.</t>
   </si>
   <si>
@@ -153,13 +149,16 @@
   </si>
   <si>
     <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed. XXX TODO: Why is gimme_boxes not part of the hello frame?</t>
+  </si>
+  <si>
+    <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +303,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -318,34 +322,34 @@
         <a:sysClr val="window" lastClr="D4D0C8"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1F497D" mc:Ignorable=""/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="EEECE1" mc:Ignorable=""/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4F81BD" mc:Ignorable=""/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0504D" mc:Ignorable=""/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="9BBB59" mc:Ignorable=""/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="8064A2" mc:Ignorable=""/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4BACC6" mc:Ignorable=""/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="F79646" mc:Ignorable=""/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable=""/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="800080" mc:Ignorable=""/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -382,6 +386,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -416,6 +421,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -497,7 +503,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
                 <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -506,7 +512,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
                 <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -515,7 +521,7 @@
         <a:effectStyle>
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
                 <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
@@ -591,14 +597,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="6.42578125" style="1" customWidth="1"/>
@@ -609,22 +615,22 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5" customHeight="1">
+    <row r="1" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="54" customHeight="1">
+    <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1">
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -644,7 +650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="50.25" customHeight="1">
+    <row r="5" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -661,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -684,7 +690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="38.25">
+    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -701,11 +707,11 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.75"/>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -725,10 +731,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -746,7 +752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18" customHeight="1">
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -766,7 +772,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="25.5" customHeight="1">
+    <row r="13" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -783,10 +789,10 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -806,7 +812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -823,12 +829,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="66" customHeight="1">
+    <row r="16" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
@@ -840,11 +846,11 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1"/>
-    <row r="18" spans="1:6" ht="16.5" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -864,8 +870,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
-    <row r="20" spans="1:6" ht="16.5" customHeight="1">
+    <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -885,7 +891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19.5" customHeight="1">
+    <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -905,7 +911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16.5" customHeight="1">
+    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -925,7 +931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -945,7 +951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16.5" customHeight="1">
+    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -965,7 +971,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="22.5" customHeight="1">
+    <row r="25" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -985,7 +991,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1">
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1005,24 +1011,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
work on untested code to handle HTTP; update protocol.xlsx
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11310"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="11880" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -144,14 +144,14 @@
     <t>reset, unicodeReason, applicationLevel?</t>
   </si>
   <si>
-    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": transportType, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": numPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks}
+    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed. XXX TODO: Why is gimme_boxes not part of the hello frame?</t>
+  </si>
+  <si>
+    <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
+  </si>
+  <si>
+    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": httpFormat, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": needPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks}
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
-  </si>
-  <si>
-    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed. XXX TODO: Why is gimme_boxes not part of the hello frame?</t>
-  </si>
-  <si>
-    <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
   </si>
 </sst>
 </file>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
@@ -846,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
docs/protocol.xlsx: (probably) minor cleanups/changes; minerva/newlink.py: change some comments
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -81,9 +81,6 @@
     <t>you_close_it</t>
   </si>
   <si>
-    <t>t_k means transport_kill</t>
-  </si>
-  <si>
     <t>Often called when the server is shutting down</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   <si>
     <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": httpFormat, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": needPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks}
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
+  </si>
+  <si>
+    <t>tk_ means transport_kill</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -622,12 +622,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -638,13 +638,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -667,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
     </row>
     <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -707,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
@@ -734,7 +734,7 @@
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -789,12 +789,12 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -846,13 +846,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -873,7 +873,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -908,12 +908,12 @@
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -948,12 +948,12 @@
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -968,27 +968,27 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove the gimme_boxes frame type; move this boolean (and the succeedsTransport argument) into the hello frame.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
   <si>
     <t>Message type</t>
   </si>
@@ -99,9 +99,6 @@
     <t>sack, seqNum, sackedList</t>
   </si>
   <si>
-    <t>gimme_boxes, succeedsTransport</t>
-  </si>
-  <si>
     <t>tk_stream_attach_failure</t>
   </si>
   <si>
@@ -141,17 +138,14 @@
     <t>reset, unicodeReason, applicationLevel?</t>
   </si>
   <si>
-    <t>gimme_boxes is sent C2S only to indicate that client wants to start receiving boxes. It is implied that server always wants to receive boxes over any existing or new transport; making the client wait for a "gimme_boxes" from the server would introduce a round trip. If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed. XXX TODO: Why is gimme_boxes not part of the hello frame?</t>
-  </si>
-  <si>
     <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
   </si>
   <si>
-    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": httpFormat, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": needPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks}
+    <t>tk_ means transport_kill</t>
+  </si>
+  <si>
+    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": httpFormat, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": needPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks, "g": succeedsTransport}. Presence of "g" means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
-  </si>
-  <si>
-    <t>tk_ means transport_kill</t>
   </si>
 </sst>
 </file>
@@ -601,7 +595,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -622,7 +616,7 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -638,13 +632,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -667,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -690,26 +684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -734,7 +709,7 @@
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -769,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -789,7 +764,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -846,13 +821,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -873,7 +848,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -893,7 +868,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -913,7 +888,7 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -933,7 +908,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -953,7 +928,7 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -973,22 +948,22 @@
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove Fn.boxes, allow only Fn.seqnum and Fn.box (applies to both S2C and C2S); rename Fn.box -> Fn.string; "bunch" received {Fn.string}s before giving them to Stream. Improve formatting of some tests.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144315"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>Message type</t>
   </si>
@@ -63,13 +63,7 @@
     <t>timestamp, timestamp_sequence_number</t>
   </si>
   <si>
-    <t>boxes, boxes</t>
-  </si>
-  <si>
     <t>This means the JSON in some frame could not be parsed. If client received corrupt frames, just make a new request.</t>
-  </si>
-  <si>
-    <t>Both parties send boxes - this is the whole point of Minerva.</t>
   </si>
   <si>
     <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
@@ -146,6 +140,15 @@
   <si>
     <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": httpFormat, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": needPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks, "g": succeedsTransport}. Presence of "g" means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
+  </si>
+  <si>
+    <t>box, string</t>
+  </si>
+  <si>
+    <t>Both parties send strings (previous boxes) - this is the whole point of Minerva.</t>
+  </si>
+  <si>
+    <t>seqnum, nextSeqNum</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="A7:F7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -616,12 +619,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -632,13 +635,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
@@ -661,7 +664,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -681,14 +684,30 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -703,13 +722,13 @@
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -729,7 +748,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -744,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,12 +783,12 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -806,7 +825,7 @@
     </row>
     <row r="16" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -821,13 +840,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -848,7 +867,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -868,7 +887,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -883,12 +902,12 @@
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -903,12 +922,12 @@
         <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -923,12 +942,12 @@
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -943,12 +962,12 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -963,12 +982,12 @@
         <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs/protocol.xlsx: update to match reality
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>Message type</t>
   </si>
@@ -63,9 +63,6 @@
     <t>timestamp, timestamp_sequence_number</t>
   </si>
   <si>
-    <t>This means the JSON in some frame could not be parsed. If client received corrupt frames, just make a new request.</t>
-  </si>
-  <si>
     <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>you_close_it</t>
   </si>
   <si>
-    <t>Often called when the server is shutting down</t>
-  </si>
-  <si>
     <t>stop_timestamps, transportNumber</t>
   </si>
   <si>
@@ -102,15 +96,9 @@
     <t>tk_frame_corruption</t>
   </si>
   <si>
-    <t>tk_intraframe_corruption</t>
-  </si>
-  <si>
     <t>tk_invalid_frame_type_or_arguments</t>
   </si>
   <si>
-    <t>tk_brb, seconds</t>
-  </si>
-  <si>
     <t>S2C Socket-like</t>
   </si>
   <si>
@@ -138,17 +126,18 @@
     <t>tk_ means transport_kill</t>
   </si>
   <si>
-    <t>helloData: {"n": transportNumber, "v: protocolVersion, "t": httpFormat, "w": requestNewStream, "i": streamId, "c": credentialsData, "p": needPaddingBytes, "r": maxReceiveBytes, "m": maxOpenTime, "o": readOnlyOnce: "a": useMyTcpAcks, "g": succeedsTransport}. Presence of "g" means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
+    <t>box, string</t>
+  </si>
+  <si>
+    <t>Both parties send strings (previous boxes) - this is the whole point of Minerva.</t>
+  </si>
+  <si>
+    <t>seqnum, nextSeqNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> transportNumber = 'tnum', protocolVersion = 'ver', httpFormat = 'format', requestNewStream = 'new', streamId = 'id', credentialsData = 'cred',  streamingResponse = 'ming', needPaddingBytes = 'pad', maxReceiveBytes = 'maxb', maxOpenTime = 'maxt', useMyTcpAcks = 'tcpack', succeedsTransport = 'eeds', lastSackSeenByClient = 'lastack'
+Presence of succeedsTransport option means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
-  </si>
-  <si>
-    <t>box, string</t>
-  </si>
-  <si>
-    <t>Both parties send strings (previous boxes) - this is the whole point of Minerva.</t>
-  </si>
-  <si>
-    <t>seqnum, nextSeqNum</t>
   </si>
 </sst>
 </file>
@@ -597,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -619,12 +608,12 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -635,19 +624,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -664,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -684,13 +673,13 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -707,7 +696,7 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -722,13 +711,13 @@
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -748,7 +737,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -763,7 +752,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -783,12 +772,12 @@
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -825,7 +814,7 @@
     </row>
     <row r="16" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -840,13 +829,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -867,7 +856,7 @@
     <row r="19" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -887,7 +876,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -902,32 +891,13 @@
         <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -942,32 +912,13 @@
         <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="2" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -982,12 +933,12 @@
         <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
When Python Minerva server's receive window overflows, kill the transport that delivered "the last straw", but don't kill the Stream; Rationales.rst: write more things
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
   <si>
     <t>Message type</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Y / N indicates whether this message is part of the spec for this direction (C2S/S2C) and mode (HTTP/Sock)</t>
   </si>
   <si>
     <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
@@ -51,25 +48,10 @@
 Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
   </si>
   <si>
-    <t>HelloFrame(helloData)</t>
-  </si>
-  <si>
-    <t>PaddingFrame(numBytes)</t>
-  </si>
-  <si>
-    <t>SeqNumFrame(nextSeqNum)</t>
-  </si>
-  <si>
-    <t>StringFrame(string)</t>
-  </si>
-  <si>
     <t>Either peer can reset if they've given up on this stream. reasonString is highly restricted to allow bytes/codepoints.</t>
   </si>
   <si>
     <t>Both peers send strings (previously "boxes") - every other frame supports this basic function. string is highly restricted to allow bytes/codepoints.</t>
-  </si>
-  <si>
-    <t>SackFrame(ackNumber, sackList)</t>
   </si>
   <si>
     <t>C2S
@@ -91,72 +73,407 @@
     <t>Idea: maybe distinct 'goodbye' and 'reset'?</t>
   </si>
   <si>
-    <t>YouCloseItFrame()</t>
-  </si>
-  <si>
-    <t>StopTimestampsFrame(transportNumber)</t>
-  </si>
-  <si>
     <t>Idea: advise_connect_bulk_transport: S2C-only message: Server indicates that client should try to establish an S2C transport more suitable for bulk transport. TODO: define this more</t>
   </si>
   <si>
-    <t>ResetFrame(
+    <t>"The next string I write to the transport will have this seqNum"</t>
+  </si>
+  <si>
+    <t>See StartTimestampsFrame</t>
+  </si>
+  <si>
+    <t>The actual timestamp payload</t>
+  </si>
+  <si>
+    <t>This error is a possible response to HelloFrame. It means transport auth failed, or streamId does not exist.</t>
+  </si>
+  <si>
+    <t>This error is a response to client sending a SackFrame that SACKed strings that server never sent. Only the server sends acked_unsent_boxes. If the client thinks server sent a bad SACK, it should send ResetFrame.</t>
+  </si>
+  <si>
+    <t>This error is a response to client sending corrupt frame octets or an overlong frame. Only server sends frame_corruption. If client received corrupt frames, it should make a new transport.</t>
+  </si>
+  <si>
+    <t>This error is a response to client sending any unknown frame, or frame with invalid arguments. Only server sends invalid_frame_type_or_arguments. Only server sends invalid_frame_type_or_arguments. If client gets an unknown frame type or bad arguments, ir should make a new transport.</t>
+  </si>
+  <si>
+    <t>Activate timestamps on a specific transport, if transport exists. Clients need timestamps to determine if a streaming connection is being buffered. It can also request them if it needs them as NOOPs to prevent an intermediary from closing the transport. Or it can request 1 timestamp if it needs an initial frame to determine how long it took to open the transport. We have a `transportNumber` argument because client may want to activate/deactivate timestamps on an existing streaming XHR transport.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TimestampFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+timestamp_sequence_number)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>StopTimestampsFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(transportNumber)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>StartTimestampsFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+transportNumber, interval, howMany)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>SackFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(ackNumber, sackList)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>ResetFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
 reasonString, applicationLevel?)</t>
-  </si>
-  <si>
-    <t>TransportKillFrame(
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>StringFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(string)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>PaddingFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(numBytes)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>SeqNumFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(nextSeqNum)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>HelloFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(helloData)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>YouCloseItFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TransportKillFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+"stream_attach_failure")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TransportKillFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+"acked_unsent_boxes")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TransportKillFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+"frame_corruption")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TransportKillFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
 "invalid_frame_type_or_arguments")</t>
-  </si>
-  <si>
-    <t>TransportKillFrame(
-"frame_corruption")</t>
-  </si>
-  <si>
-    <t>TransportKillFrame(
-"acked_unsent_boxes")</t>
-  </si>
-  <si>
-    <t>TransportKillFrame(
-"stream_attach_failure")</t>
-  </si>
-  <si>
-    <t>TimestampFrame(
-timestamp_sequence_number)</t>
-  </si>
-  <si>
-    <t>"The next string I write to the transport will have this seqNum"</t>
-  </si>
-  <si>
-    <t>StartTimestampsFrame(
-transportNumber, interval, howMany)</t>
-  </si>
-  <si>
-    <t>See StartTimestampsFrame</t>
-  </si>
-  <si>
-    <t>The actual timestamp payload</t>
-  </si>
-  <si>
-    <t>This error is a possible response to HelloFrame. It means transport auth failed, or streamId does not exist.</t>
-  </si>
-  <si>
-    <t>This error is a response to client sending a SackFrame that SACKed strings that server never sent. Only the server sends acked_unsent_boxes. If the client thinks server sent a bad SACK, it should send ResetFrame.</t>
-  </si>
-  <si>
-    <t>This error is a response to client sending corrupt frame octets or an overlong frame. Only server sends frame_corruption. If client received corrupt frames, it should make a new transport.</t>
-  </si>
-  <si>
-    <t>This error is a response to client sending any unknown frame, or frame with invalid arguments. Only server sends invalid_frame_type_or_arguments. Only server sends invalid_frame_type_or_arguments. If client gets an unknown frame type or bad arguments, ir should make a new transport.</t>
-  </si>
-  <si>
-    <t>Activate timestamps on a specific transport, if transport exists. Clients need timestamps to determine if a streaming connection is being buffered. It can also request them if it needs them as NOOPs to prevent an intermediary from closing the transport. Or it can request 1 timestamp if it needs an initial frame to determine how long it took to open the transport. We have a `transportNumber` argument because client may want to activate/deactivate timestamps on an existing streaming XHR transport.</t>
+    </r>
+  </si>
+  <si>
+    <t>Gray background means not yet implemented</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> /</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> indicates whether this message is part of the spec for this direction (C2S/S2C) and mode (HTTP/Sock)</t>
+    </r>
+  </si>
+  <si>
+    <t>This error is a response to client that has caused the server's receive window to overflow by sending strings that cannot be delivered. Later, client can connect a new transport and send deliverable strings. Only server sends overflowing_rwin. If client's receive window is overflowing, it should make a new transport and write a SackFrame.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TransportKillFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+"rwin_overflow")</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,13 +494,33 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -198,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -212,11 +549,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -598,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -615,13 +978,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -629,16 +995,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>3</v>
@@ -646,300 +1012,320 @@
     </row>
     <row r="4" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>39</v>
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
+      <c r="A11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>34</v>
+      <c r="A12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A27:A1048576 A1:XFD2 B26:XFD1048576 G3:XFD25 A21:F21 A23:F24 A3:F18">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
JS and Py Minerva: Add StreamCreatedFrame. Soon server will be updated to send it after a Stream is created successfully. Client needs to know about this important state change.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
   <si>
     <t>Message type</t>
   </si>
@@ -467,6 +466,12 @@
       <t>(
 "rwin_overflow")</t>
     </r>
+  </si>
+  <si>
+    <t>StreamCreated()</t>
+  </si>
+  <si>
+    <t>Sent to indicate that a Stream has been successfully created. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
   </si>
 </sst>
 </file>
@@ -535,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -561,11 +566,28 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -962,7 +984,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1031,208 +1053,208 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="B7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="B11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="B12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
+      <c r="B13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>2</v>
@@ -1247,66 +1269,86 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="B17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="B19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1321,7 +1363,15 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A27:A1048576 A1:XFD2 B26:XFD1048576 G3:XFD25 A21:F21 A23:F24 A3:F18">
+  <conditionalFormatting sqref="A27:A1048576 A1:XFD2 B26:XFD1048576 G3:XFD25 A21:F21 A23:F24 A3:F4 A6:F19">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:F5">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
JS and Py Minerva: add a StreamStatusFrame which will be used by server to send `lastSackSeenByServer` information; client.js: add a TODO
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
   <si>
     <t>Message type</t>
   </si>
@@ -36,15 +36,7 @@
     <t>There's a difference between "client" and "server" because client is: initiating all the connections, generally has more memory/CPU time/TIME_WAIT slots than server, and because the server doesn't really care about all the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch.</t>
   </si>
   <si>
-    <t>Both parties need to sack often to free memory in their peer's box queue</t>
-  </si>
-  <si>
     <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> transportNumber = 'tnum', protocolVersion = 'ver', httpFormat = 'format', requestNewStream = 'new', streamId = 'id', credentialsData = 'cred',  streamingResponse = 'ming', needPaddingBytes = 'pad', maxReceiveBytes = 'maxb', maxOpenTime = 'maxt', useMyTcpAcks = 'tcpack', succeedsTransport = 'eeds', lastSackSeenByClient = 'lastack'
-Presence of succeedsTransport option means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
-Only C2S because hello is used by the client to identify itself to the server, and set critical transport parameters. XXX TODO: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
   </si>
   <si>
     <t>Either peer can reset if they've given up on this stream. reasonString is highly restricted to allow bytes/codepoints.</t>
@@ -69,9 +61,6 @@
 Sock</t>
   </si>
   <si>
-    <t>Idea: maybe distinct 'goodbye' and 'reset'?</t>
-  </si>
-  <si>
     <t>Idea: advise_connect_bulk_transport: S2C-only message: Server indicates that client should try to establish an S2C transport more suitable for bulk transport. TODO: define this more</t>
   </si>
   <si>
@@ -172,27 +161,6 @@
         <rFont val="Tahoma"/>
         <family val="2"/>
       </rPr>
-      <t>SackFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(ackNumber, sackList)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
       <t>ResetFrame</t>
     </r>
     <r>
@@ -472,6 +440,66 @@
   </si>
   <si>
     <t>StreamCreatedFrame()</t>
+  </si>
+  <si>
+    <t>Both parties need to sack often to free memory in their peer's send queue</t>
+  </si>
+  <si>
+    <t>Idea: maybe distinct 'shutdown' and 'reset'?</t>
+  </si>
+  <si>
+    <t>HelloFrame arguments: transportNumber = 'tnum', protocolVersion = 'ver', httpFormat = 'format', requestNewStream = 'new', streamId = 'id', credentialsData = 'cred',  streamingResponse = 'ming', needPaddingBytes = 'pad', maxReceiveBytes = 'maxb', maxOpenTime = 'maxt', useMyTcpAcks = 'tcpack', succeedsTransport = 'eeds', lastSackSeenByClient = 'lastack'
+Presence of succeedsTransport option means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
+Idea: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
+  </si>
+  <si>
+    <t>Used to authenticate each transport that connects to the Minerva server. C2S only because HelloFrame is used by the client to identify itself to the server, and set critical transport parameters.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>SackFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(sack)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>StreamStatusFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+lastSackSeenByServer)</t>
+    </r>
+  </si>
+  <si>
+    <t>Used to tell the client the `lastSackSeenByServer` before server closes the transport. Client uses this information to decide whether it needs to send a SackFrame again. S2C only. Client reports its `lastSackSeenByClient` in the HelloFrame.</t>
   </si>
 </sst>
 </file>
@@ -573,7 +601,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -981,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1001,10 +1043,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
@@ -1017,24 +1059,24 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>1</v>
@@ -1049,12 +1091,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -1069,12 +1111,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -1094,7 +1136,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -1109,12 +1151,12 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>1</v>
@@ -1129,12 +1171,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>1</v>
@@ -1149,12 +1191,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>1</v>
@@ -1169,112 +1211,112 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>2</v>
@@ -1289,12 +1331,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>2</v>
@@ -1309,12 +1351,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>2</v>
@@ -1329,41 +1371,74 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>16</v>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A27:A1048576 A1:XFD2 B26:XFD1048576 G3:XFD25 A21:F21 A23:F24 A3:F4 A6:F19">
+  <conditionalFormatting sqref="A1:XFD2 B26:XFD1048576 G3:XFD25 A3:F4 A27 A30:A1048576 A23:F24 A6:F10 A12:F21">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:F5">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -1371,7 +1446,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:F5">
+  <conditionalFormatting sqref="A11:F11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Py Minerva: make explicit that StreamCreatedFrame is now always the first frame sent, if the frame is sent at all. JS Minerva: remove hack for previous behavior where SackFrame (maybe even other frames?) might have been sent before StreamCreatedFrame.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -436,9 +436,6 @@
     </r>
   </si>
   <si>
-    <t>Sent to indicate that a Stream has been successfully created. Sent over *every* transport with `requestNewStream`, so it may be sent one or more times per Stream. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
-  </si>
-  <si>
     <t>StreamCreatedFrame()</t>
   </si>
   <si>
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>Used to tell the client the `lastSackSeenByServer` before server closes the transport. Client uses this information to decide whether it needs to send a SackFrame again. S2C only. Client reports its `lastSackSeenByClient` in the HelloFrame.</t>
+  </si>
+  <si>
+    <t>Sent to indicate that a Stream has been successfully created. This is the first frame sent over *every* sucessfully-authenticated transport with `requestNewStream`, so it may be sent over more than one in transport. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1091,12 +1091,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>1</v>
@@ -1211,27 +1211,27 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
@@ -1416,12 +1416,12 @@
     </row>
     <row r="22" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
docs/protocol.xlsx: fix document to match reality: acked_unsent_boxes -> acked_unsent_strings
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -320,28 +320,6 @@
         <family val="2"/>
       </rPr>
       <t>(
-"acked_unsent_boxes")</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>TransportKillFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(
 "frame_corruption")</t>
     </r>
   </si>
@@ -500,6 +478,28 @@
     <t>HelloFrame arguments: transportNumber = 'tnum', protocolVersion = 'ver', httpFormat = 'format', requestNewStream = 'new', streamId = 'id', credentialsData = 'cred',  streamingResponse = 'ming', needPaddingBytes = 'pad', maxReceiveBytes = 'maxb', maxOpenTime = 'maxt', useMyTcpAcks = 'tcpack', succeedsTransport = 'eeds', sack = 'sack', lastSackSeenByClient = 'lastack'
 Presence of succeedsTransport option means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
 Idea: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TransportKillFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+"acked_unsent_strings")</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1043,10 +1043,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
@@ -1091,12 +1091,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>1</v>
@@ -1211,27 +1211,27 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
@@ -1336,7 +1336,7 @@
     </row>
     <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>2</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>2</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>2</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>2</v>
@@ -1411,17 +1411,17 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Py Minerva: Implement maxOpenTime on server. Also:
 * maxOpenTime is now measured in milliseconds, not seconds.

 * Update clients for the above change.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -601,21 +601,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -1025,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1431,26 +1417,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD2 B26:XFD1048576 G3:XFD25 A3:F4 A27 A30:A1048576 A23:F24 A6:F10 A12:F21">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:F5">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:F11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
docs/protocol.xlsx: clarify text about codepoint restrictions
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -39,12 +39,6 @@
     <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends you_close_it over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
   </si>
   <si>
-    <t>Either peer can reset if they've given up on this stream. reasonString is highly restricted to allow bytes/codepoints.</t>
-  </si>
-  <si>
-    <t>Both peers send strings (previously "boxes") - every other frame supports this basic function. string is highly restricted to allow bytes/codepoints.</t>
-  </si>
-  <si>
     <t>C2S
 HTTP</t>
   </si>
@@ -500,6 +494,12 @@
   </si>
   <si>
     <t>This error is a response to client sending any unknown frame, or frame with invalid arguments. Only server sends invalid_frame_type_or_arguments. Only server sends invalid_frame_type_or_arguments. If client gets an unknown frame type or bad arguments, it should make a new transport.</t>
+  </si>
+  <si>
+    <t>Both peers send strings (previously "boxes") - every other frame supports this basic function. `string` is restricted to the base "restricted string" codepoints.</t>
+  </si>
+  <si>
+    <t>Either peer can reset if they've given up on this stream. `reasonString` is restricted to the base "restricted string" codepoints.</t>
   </si>
 </sst>
 </file>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1029,10 +1029,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
@@ -1045,16 +1045,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>3</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>1</v>
@@ -1077,12 +1077,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -1097,12 +1097,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -1137,12 +1137,12 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>1</v>
@@ -1157,12 +1157,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>1</v>
@@ -1177,12 +1177,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>1</v>
@@ -1197,12 +1197,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>2</v>
@@ -1217,12 +1217,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>1</v>
@@ -1237,12 +1237,12 @@
         <v>2</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>1</v>
@@ -1257,12 +1257,12 @@
         <v>2</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>2</v>
@@ -1277,12 +1277,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>2</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>2</v>
@@ -1317,12 +1317,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>2</v>
@@ -1337,12 +1337,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>2</v>
@@ -1357,12 +1357,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>2</v>
@@ -1377,12 +1377,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>2</v>
@@ -1397,22 +1397,22 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs/protocol.xlsx: remove some out-of-data information
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -408,98 +408,98 @@
     <t>Sent to indicate that a Stream has been successfully created. This is the first frame sent over *every* sucessfully-authenticated transport with `requestNewStream`, so it may be sent over more than one in transport. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
   </si>
   <si>
-    <t>HelloFrame arguments: transportNumber = 'tnum', protocolVersion = 'ver', httpFormat = 'format', requestNewStream = 'new', streamId = 'id', credentialsData = 'cred',  streamingResponse = 'ming', needPaddingBytes = 'pad', maxReceiveBytes = 'maxb', maxOpenTime = 'maxt', useMyTcpAcks = 'tcpack', succeedsTransport = 'eeds', sack = 'sack', lastSackSeenByClient = 'lastack'
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>TransportKillFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(
+"acked_unsent_strings")</t>
+    </r>
+  </si>
+  <si>
+    <t>This error is a response to client sending any unknown frame, or frame with invalid arguments. Only server sends invalid_frame_type_or_arguments. Only server sends invalid_frame_type_or_arguments. If client gets an unknown frame type or bad arguments, it should make a new transport.</t>
+  </si>
+  <si>
+    <t>Both peers send strings (previously "boxes") - every other frame supports this basic function. `string` is restricted to the base "restricted string" codepoints.</t>
+  </si>
+  <si>
+    <t>Either peer can reset if they've given up on this stream. `reasonString` is restricted to the base "restricted string" codepoints.</t>
+  </si>
+  <si>
+    <t>Used to tell the client the `lastSackSeenByServer` before server closes the transport. Client uses this information to decide whether it needs to send a SackFrame. S2C only. Client also sends similar information to server, but it does so with `lastSackSeenByClient` in the HelloFrame.</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Why does server send TransportKillFrames, but client does not? Because the server doesn't really care about the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch later.</t>
+  </si>
+  <si>
+    <t>Gray background means not yet implemented.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> /</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> indicates whether this message is part of the spec for this direction (C2S/S2C) and mode (HTTP/Sock).</t>
+    </r>
+  </si>
+  <si>
+    <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends YouCloseItFrame over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
+  </si>
+  <si>
+    <t>This error is a possible response to HelloFrame. It means transport authentication failed, or streamId does not exist.</t>
+  </si>
+  <si>
+    <t>HelloFrame arguments are documented in frames.py and frames.js
 Presence of succeedsTransport option means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
 Idea: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>TransportKillFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(
-"acked_unsent_strings")</t>
-    </r>
-  </si>
-  <si>
-    <t>This error is a response to client sending any unknown frame, or frame with invalid arguments. Only server sends invalid_frame_type_or_arguments. Only server sends invalid_frame_type_or_arguments. If client gets an unknown frame type or bad arguments, it should make a new transport.</t>
-  </si>
-  <si>
-    <t>Both peers send strings (previously "boxes") - every other frame supports this basic function. `string` is restricted to the base "restricted string" codepoints.</t>
-  </si>
-  <si>
-    <t>Either peer can reset if they've given up on this stream. `reasonString` is restricted to the base "restricted string" codepoints.</t>
-  </si>
-  <si>
-    <t>Used to tell the client the `lastSackSeenByServer` before server closes the transport. Client uses this information to decide whether it needs to send a SackFrame. S2C only. Client also sends similar information to server, but it does so with `lastSackSeenByClient` in the HelloFrame.</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Why does server send TransportKillFrames, but client does not? Because the server doesn't really care about the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch later.</t>
-  </si>
-  <si>
-    <t>Gray background means not yet implemented.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> /</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> indicates whether this message is part of the spec for this direction (C2S/S2C) and mode (HTTP/Sock).</t>
-    </r>
-  </si>
-  <si>
-    <t>In S2C context: This is useful when server wants client to do active close on the TCP socket for this transport (usually, to avoid having TIME_WAIT sockets). If server sends YouCloseItFrame over an HTTP transport, client must try to close the HTTP connection. (usually with xhrObject.abort() or removing an iframe)</t>
-  </si>
-  <si>
-    <t>This error is a possible response to HelloFrame. It means transport authentication failed, or streamId does not exist.</t>
   </si>
 </sst>
 </file>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1029,12 +1029,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1314,12 +1314,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>2</v>
@@ -1374,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
@@ -1397,9 +1397,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
     </row>
     <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="F26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JS and Py Minerva: Remove PaddingFrame and replace it with a CommentFrame, which does decode the actual comment in the frame, and is only equal to CommentFrames with the same comment.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -27,9 +27,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
-  </si>
-  <si>
     <t>C2S
 HTTP</t>
   </si>
@@ -172,27 +169,6 @@
         <family val="2"/>
       </rPr>
       <t>(string)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>PaddingFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(numBytes)</t>
     </r>
   </si>
   <si>
@@ -500,6 +476,30 @@
     <t>HelloFrame arguments are documented in frames.py and frames.js
 Presence of succeedsTransport option means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
 Idea: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>CommentFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(comment)</t>
+    </r>
+  </si>
+  <si>
+    <t>CommentFrame is used for HTTP anti-script-inclusion preamble, padding, and heartbeats.  Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
   </si>
 </sst>
 </file>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1029,12 +1029,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1042,24 +1042,24 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>1</v>
@@ -1074,12 +1074,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -1094,12 +1094,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -1114,12 +1114,12 @@
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>1</v>
@@ -1134,12 +1134,12 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>1</v>
@@ -1154,12 +1154,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>1</v>
@@ -1174,12 +1174,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>1</v>
@@ -1194,12 +1194,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>2</v>
@@ -1214,12 +1214,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>1</v>
@@ -1234,12 +1234,12 @@
         <v>2</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>1</v>
@@ -1254,12 +1254,12 @@
         <v>2</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>2</v>
@@ -1274,12 +1274,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>2</v>
@@ -1294,12 +1294,12 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>2</v>
@@ -1314,12 +1314,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>2</v>
@@ -1334,12 +1334,12 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>2</v>
@@ -1354,12 +1354,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>2</v>
@@ -1374,12 +1374,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>2</v>
@@ -1394,27 +1394,27 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="F26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs/protocol.xlsx: fix a mistake: CommentFrame is sent over `S2C Sock` as well.
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Don't document StartTimestampsFrame etc which do not exist and don't need to exist (because we have CommentFrame for heartbeats)
</commit_message>
<xml_diff>
--- a/docs/protocol.xlsx
+++ b/docs/protocol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t>Message type</t>
   </si>
@@ -49,84 +49,10 @@
     <t>"The next string I write to the transport will have this seqNum"</t>
   </si>
   <si>
-    <t>See StartTimestampsFrame</t>
-  </si>
-  <si>
-    <t>The actual timestamp payload</t>
-  </si>
-  <si>
     <t>This error is a response to client sending a SackFrame that SACKed strings that server never sent. Only the server sends acked_unsent_boxes. If the client thinks server sent a bad SACK, it should send ResetFrame.</t>
   </si>
   <si>
     <t>This error is a response to client sending corrupt frame octets or an overlong frame. Only server sends frame_corruption. If client received corrupt frames, it should make a new transport.</t>
-  </si>
-  <si>
-    <t>Activate timestamps on a specific transport, if transport exists. Clients need timestamps to determine if a streaming connection is being buffered. It can also request them if it needs them as NOOPs to prevent an intermediary from closing the transport. Or it can request 1 timestamp if it needs an initial frame to determine how long it took to open the transport. We have a `transportNumber` argument because client may want to activate/deactivate timestamps on an existing streaming XHR transport.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>TimestampFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(
-timestamp_sequence_number)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>StopTimestampsFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(transportNumber)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>StartTimestampsFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(
-transportNumber, interval, howMany)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -422,9 +348,6 @@
   </si>
   <si>
     <t>Why does server send TransportKillFrames, but client does not? Because the server doesn't really care about the client's problems with decoding frames. Server is still interested in this "problems" data, so it could be sent in a batch later.</t>
-  </si>
-  <si>
-    <t>Gray background means not yet implemented.</t>
   </si>
   <si>
     <r>
@@ -542,18 +465,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -568,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -582,16 +499,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1009,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1029,13 +937,11 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F2" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1054,83 +960,83 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1139,286 +1045,226 @@
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="F22" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="F26" s="2" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B27:XFD1048576 A30:A1048576 A23:F24 A6:F10 A12:F21 G2:XFD26 A27 B26:F26 B1:XFD1 A2:F4">
+  <conditionalFormatting sqref="B24:XFD1048576 A27:A1048576 A20:F21 A6:F10 A24 B23:F23 B1:XFD1 A2:F4 A12:F18 G2:XFD23">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"N"</formula>
     </cfRule>
@@ -1444,6 +1290,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <webPublishItems count="1">
+    <webPublishItem id="10526" divId="protocol_10526" sourceType="sheet" destinationFile="L:\home\at\Projects\Minerva\docs\protocol.htm" autoRepublish="1"/>
+  </webPublishItems>
 </worksheet>
 </file>
 

</xml_diff>